<commit_message>
updated case to include changes from demo of October 2016
</commit_message>
<xml_diff>
--- a/CaseStudies/SimulinkOpal/SYMP2015_R2013a/relay_settings_10272015.xlsx
+++ b/CaseStudies/SimulinkOpal/SYMP2015_R2013a/relay_settings_10272015.xlsx
@@ -474,7 +474,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,13 +523,13 @@
         <v>2500</v>
       </c>
       <c r="E2" s="6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F2" s="6">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G2" s="6">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -658,7 +658,7 @@
         <v>40000</v>
       </c>
       <c r="D8" s="5">
-        <v>5000</v>
+        <v>9000</v>
       </c>
       <c r="E8" s="6">
         <v>5</v>
@@ -681,7 +681,7 @@
         <v>30000</v>
       </c>
       <c r="D9" s="5">
-        <v>8000</v>
+        <v>10000</v>
       </c>
       <c r="E9" s="6">
         <v>5</v>

</xml_diff>